<commit_message>
Atualização do backlog de requisitos com base na discussão do grupo
</commit_message>
<xml_diff>
--- a/Backlog HerpSafe/Produck backlog.xlsx
+++ b/Backlog HerpSafe/Produck backlog.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF23BFE-BD73-4713-A20C-D0E36BAB40A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46BAC1F4-1C84-45BD-BB05-3DAD47173D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5205" windowWidth="29040" windowHeight="15720" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
-    <sheet name="Legenda" sheetId="6" r:id="rId2"/>
-    <sheet name="Sugestões para requisitos" sheetId="5" r:id="rId3"/>
-    <sheet name="Fibonacci" sheetId="4" r:id="rId4"/>
+    <sheet name="Fibonacci por Sprint" sheetId="7" r:id="rId2"/>
+    <sheet name="Legenda" sheetId="6" r:id="rId3"/>
+    <sheet name="Sugestões para requisitos" sheetId="5" r:id="rId4"/>
+    <sheet name="Fibonacci" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$B$1:$K$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$B$1:$L$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="161">
   <si>
     <t>Tipo</t>
   </si>
@@ -477,13 +478,75 @@
   </si>
   <si>
     <t>Se 'Entregável', informar o nome da disciplina associada. Se 'Desejável', informar se requisito é funcional ou não funcional</t>
+  </si>
+  <si>
+    <r>
+      <t>Sprint</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.#</t>
+    </r>
+  </si>
+  <si>
+    <t>SP2.3</t>
+  </si>
+  <si>
+    <t>SP2.2</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Baixa</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>SP2.1</t>
+  </si>
+  <si>
+    <t>SP2.4</t>
+  </si>
+  <si>
+    <t>Validação com a Vivian</t>
+  </si>
+  <si>
+    <t>Site institucional revamp</t>
+  </si>
+  <si>
+    <t>Alterar o site com base nas alterações no protótipo</t>
+  </si>
+  <si>
+    <t>Checar detalhes referentes a modelagem do banco de dados</t>
+  </si>
+  <si>
+    <t>Validar Diagrama da solução técnica</t>
+  </si>
+  <si>
+    <t>Checar se diagrama da solução técnica está de acordo com o modelo de ISO</t>
+  </si>
+  <si>
+    <t>Divisão</t>
+  </si>
+  <si>
+    <t>SP3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,6 +566,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -555,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -581,41 +653,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1036,11 +1081,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
-  <dimension ref="B1:K52"/>
+  <dimension ref="B1:L55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.1" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1055,11 +1100,12 @@
     <col min="8" max="8" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="34" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="11.28515625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
@@ -1088,25 +1134,32 @@
         <v>1</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="str">
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4">
         <f>IFERROR(VLOOKUP(E2,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G2" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1114,28 +1167,35 @@
         <v>4</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>114</v>
+        <v>60</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="str">
+      <c r="E3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="4">
         <f>IFERROR(VLOOKUP(E3,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G3" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
@@ -1143,28 +1203,35 @@
         <v>4</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>116</v>
+        <v>61</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="str">
+      <c r="E4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="4">
         <f>IFERROR(VLOOKUP(E4,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G4" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H4" s="4" t="s">
         <v>13</v>
       </c>
@@ -1172,86 +1239,107 @@
         <v>4</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="str">
+      <c r="E5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="4">
         <f>IFERROR(VLOOKUP(E5,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="str">
+      <c r="E6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="4">
         <f>IFERROR(VLOOKUP(E6,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G6" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="str">
+      <c r="E7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="4">
         <f>IFERROR(VLOOKUP(E7,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1259,28 +1347,35 @@
         <v>5</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>120</v>
+        <v>65</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="str">
+      <c r="E8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="4">
         <f>IFERROR(VLOOKUP(E8,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G8" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H8" s="4" t="s">
         <v>13</v>
       </c>
@@ -1288,28 +1383,35 @@
         <v>7</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="str">
+      <c r="E9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="4">
         <f>IFERROR(VLOOKUP(E9,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G9" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1317,28 +1419,35 @@
         <v>7</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="str">
+      <c r="E10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="4">
         <f>IFERROR(VLOOKUP(E10,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G10" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1346,57 +1455,71 @@
         <v>7</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="str">
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="4">
         <f>IFERROR(VLOOKUP(E11,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4" t="str">
+      <c r="E12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="4">
         <f>IFERROR(VLOOKUP(E12,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G12" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1404,28 +1527,35 @@
         <v>9</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="str">
+      <c r="E13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="4">
         <f>IFERROR(VLOOKUP(E13,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G13" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1433,28 +1563,35 @@
         <v>9</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4" t="str">
+      <c r="E14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="4">
         <f>IFERROR(VLOOKUP(E14,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G14" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1462,28 +1599,35 @@
         <v>21</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4" t="str">
+      <c r="E15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="4">
         <f>IFERROR(VLOOKUP(E15,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G15" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1491,86 +1635,107 @@
         <v>21</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>128</v>
+        <v>71</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4" t="str">
+      <c r="E16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="4">
         <f>IFERROR(VLOOKUP(E16,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G16" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>129</v>
+        <v>71</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4" t="str">
+      <c r="E17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="4">
         <f>IFERROR(VLOOKUP(E17,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G17" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="H17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4" t="str">
+      <c r="E18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4">
         <f>IFERROR(VLOOKUP(E18,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G18" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="H18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1581,54 +1746,68 @@
         <v>22</v>
       </c>
       <c r="K18" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>57</v>
+        <v>125</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4" t="str">
+      <c r="E19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="4">
         <f>IFERROR(VLOOKUP(E19,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G19" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="H19" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4" t="str">
+      <c r="E20" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="4">
         <f>IFERROR(VLOOKUP(E20,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G20" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H20" s="4" t="s">
         <v>13</v>
       </c>
@@ -1636,115 +1815,143 @@
         <v>4</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>61</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="str">
+      <c r="E21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="4">
         <f>IFERROR(VLOOKUP(E21,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G21" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4" t="str">
+      <c r="E22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="4">
         <f>IFERROR(VLOOKUP(E22,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G22" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4" t="str">
+      <c r="E23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="4">
         <f>IFERROR(VLOOKUP(E23,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G23" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4" t="str">
+      <c r="E24" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F24" s="4">
         <f>IFERROR(VLOOKUP(E24,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G24" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H24" s="4" t="s">
         <v>13</v>
       </c>
@@ -1752,434 +1959,539 @@
         <v>5</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K24" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4" t="str">
+      <c r="E25" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="4">
         <f>IFERROR(VLOOKUP(E25,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G25" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="H25" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="4">
+        <f>IFERROR(VLOOKUP(E26,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4" t="str">
-        <f>IFERROR(VLOOKUP(E26,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="H26" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4" t="str">
+      <c r="E27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="4">
         <f>IFERROR(VLOOKUP(E27,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G27" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H27" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>14</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4" t="str">
+      <c r="E28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="4">
         <f>IFERROR(VLOOKUP(E28,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G28" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="4">
+        <f>IFERROR(VLOOKUP(E29,Fibonacci!D:E,2,0),"")</f>
+        <v>13</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F30" s="4">
+        <f>IFERROR(VLOOKUP(E30,Fibonacci!D:E,2,0),"")</f>
+        <v>8</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F31" s="4">
+        <f>IFERROR(VLOOKUP(E31,Fibonacci!D:E,2,0),"")</f>
+        <v>5</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="8" t="s">
+      <c r="J31" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L31" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="4">
+        <f>IFERROR(VLOOKUP(E32,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4" t="str">
-        <f>IFERROR(VLOOKUP(E29,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4" t="str">
-        <f>IFERROR(VLOOKUP(E30,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4" t="str">
-        <f>IFERROR(VLOOKUP(E31,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4" t="str">
-        <f>IFERROR(VLOOKUP(E32,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H32" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4" t="str">
+      <c r="E33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="4">
         <f>IFERROR(VLOOKUP(E33,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G33" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H33" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>32</v>
+        <v>77</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4" t="str">
+      <c r="E34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="4">
         <f>IFERROR(VLOOKUP(E34,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G34" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H34" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>11</v>
+        <v>154</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>71</v>
+        <v>155</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4" t="str">
+      <c r="E35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F35" s="4">
         <f>IFERROR(VLOOKUP(E35,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G35" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H35" s="4" t="s">
         <v>13</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L35" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4" t="str">
+      <c r="E36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="4">
         <f>IFERROR(VLOOKUP(E36,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G36" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H36" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>95</v>
+        <v>158</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4" t="str">
+      <c r="E37" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="4">
         <f>IFERROR(VLOOKUP(E37,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G37" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H37" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4" t="str">
+        <v>53</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F38" s="4">
         <f>IFERROR(VLOOKUP(E38,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G38" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H38" s="4" t="s">
-        <v>51</v>
+        <v>13</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>130</v>
+        <v>22</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4" t="str">
+      <c r="E39" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F39" s="4">
         <f>IFERROR(VLOOKUP(E39,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G39" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H39" s="4" t="s">
         <v>51</v>
       </c>
@@ -2187,28 +2499,35 @@
         <v>113</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K39" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L39" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4" t="str">
+        <v>89</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="4">
         <f>IFERROR(VLOOKUP(E40,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G40" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H40" s="4" t="s">
         <v>51</v>
       </c>
@@ -2216,28 +2535,35 @@
         <v>113</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L40" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4" t="str">
+        <v>90</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="4">
         <f>IFERROR(VLOOKUP(E41,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G41" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H41" s="4" t="s">
         <v>51</v>
       </c>
@@ -2245,28 +2571,35 @@
         <v>113</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K41" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L41" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4" t="str">
+      <c r="E42" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="4">
         <f>IFERROR(VLOOKUP(E42,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G42" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="H42" s="4" t="s">
         <v>51</v>
       </c>
@@ -2274,28 +2607,35 @@
         <v>113</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L42" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4" t="str">
+        <v>53</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="4">
         <f>IFERROR(VLOOKUP(E43,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G43" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H43" s="4" t="s">
         <v>51</v>
       </c>
@@ -2303,28 +2643,35 @@
         <v>113</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K43" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L43" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4" t="str">
+        <v>89</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="4">
         <f>IFERROR(VLOOKUP(E44,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G44" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="H44" s="4" t="s">
         <v>51</v>
       </c>
@@ -2332,28 +2679,35 @@
         <v>113</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K44" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L44" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="8" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4" t="str">
+        <v>89</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="4">
         <f>IFERROR(VLOOKUP(E45,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G45" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>148</v>
+      </c>
       <c r="H45" s="4" t="s">
         <v>51</v>
       </c>
@@ -2361,115 +2715,143 @@
         <v>113</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K45" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L45" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4" t="str">
+      <c r="E46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="4">
         <f>IFERROR(VLOOKUP(E46,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G46" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H46" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K46" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L46" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="8" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4" t="str">
+      <c r="E47" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F47" s="4">
         <f>IFERROR(VLOOKUP(E47,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G47" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H47" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K47" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L47" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="8" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4" t="str">
+      <c r="E48" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" s="4">
         <f>IFERROR(VLOOKUP(E48,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G48" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H48" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K48" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L48" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4" t="str">
+      <c r="E49" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" s="4">
         <f>IFERROR(VLOOKUP(E49,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G49" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H49" s="4" t="s">
         <v>51</v>
       </c>
@@ -2477,28 +2859,35 @@
         <v>104</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K49" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L49" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4" t="str">
+        <v>90</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="4">
         <f>IFERROR(VLOOKUP(E50,Fibonacci!D:E,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="G50" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>149</v>
+      </c>
       <c r="H50" s="4" t="s">
         <v>51</v>
       </c>
@@ -2506,38 +2895,150 @@
         <v>104</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="K50" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L50" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="7" t="s">
+    <row r="51" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" s="4">
+        <f>IFERROR(VLOOKUP(E51,Fibonacci!D:E,2,0),"")</f>
+        <v>8</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K51" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F52" s="4">
+        <f>IFERROR(VLOOKUP(E52,Fibonacci!D:E,2,0),"")</f>
+        <v>13</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J52" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="4">
+        <f>IFERROR(VLOOKUP(E53,Fibonacci!D:E,2,0),"")</f>
+        <v>8</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="7" t="s">
         <v>41</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:K50" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K50">
-      <sortCondition descending="1" ref="J1:J50"/>
+  <autoFilter ref="B1:L53" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L53">
+      <sortCondition ref="K1:K53"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Backlog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5EF24D9-CB2D-4BDC-89A1-7AFACDE7C990}">
           <x14:formula1>
             <xm:f>Fibonacci!$D$7:$D$11</xm:f>
@@ -2551,6 +3052,85 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B7D321-581D-4B64-AD81-A8A61543E901}">
+  <dimension ref="F7:G15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5">
+        <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F9,'Product Backlog'!F:F)</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G10" s="5">
+        <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F10,'Product Backlog'!F:F)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G11" s="5">
+        <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F11,'Product Backlog'!F:F)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="5">
+        <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F12,'Product Backlog'!F:F)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G13" s="5">
+        <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F13,'Product Backlog'!F:F)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="G14" s="5">
+        <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F14,'Product Backlog'!F:F)</f>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="6:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{148829FE-DA75-4191-B2D8-E745EAD2677E}">
   <dimension ref="B3:C14"/>
   <sheetViews>
@@ -2647,13 +3227,13 @@
     <row r="14" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="B13">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>"Backlog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2661,7 +3241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56EC897-511D-459E-B2A6-5083809C3FA0}">
   <dimension ref="B1:K4"/>
   <sheetViews>
@@ -2745,25 +3325,14 @@
     </row>
     <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+  <conditionalFormatting sqref="K2:K3">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Backlog"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Pendente"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
-      <formula>"Concluído"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"Backlog"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"Pendente"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Concluído"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2771,12 +3340,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B8A3BF-F154-4F80-A5B1-DCA44757EF3D}">
   <dimension ref="D5:E12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="D6" sqref="D6:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Atualização final do backlog de requisitos
</commit_message>
<xml_diff>
--- a/Backlog HerpSafe/Produck backlog.xlsx
+++ b/Backlog HerpSafe/Produck backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46BAC1F4-1C84-45BD-BB05-3DAD47173D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E89BF6-0D29-46CE-9988-B0863E024C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5205" windowWidth="29040" windowHeight="15720" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Fibonacci" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$B$1:$L$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$B$1:$L$55</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="165">
   <si>
     <t>Tipo</t>
   </si>
@@ -51,36 +51,18 @@
     <t>Sprint</t>
   </si>
   <si>
-    <t>Projeto criado e configrado no GitHub</t>
-  </si>
-  <si>
-    <t>Tela de simulador financeiro (individual)</t>
-  </si>
-  <si>
     <t>Pesquisa e Inovação</t>
   </si>
   <si>
     <t>Algoritmos</t>
   </si>
   <si>
-    <t>Requisitos populados na ferramenta</t>
-  </si>
-  <si>
     <t>Tecnologia da Informação</t>
   </si>
   <si>
-    <t>Tabelas criadas no MySQL - Protótipo individual</t>
-  </si>
-  <si>
     <t>Banco de Dados</t>
   </si>
   <si>
-    <t>Ligar Arduino</t>
-  </si>
-  <si>
-    <t>Linux instalado em VM local</t>
-  </si>
-  <si>
     <t>Introdução a Sistemas Operacionais</t>
   </si>
   <si>
@@ -90,84 +72,12 @@
     <t>SP1</t>
   </si>
   <si>
-    <t>Atividades organizadas na ferramenta de gestão (Sprints/Atividades)</t>
-  </si>
-  <si>
-    <t>Backlog da sprint (Demanda, pontuação, prioridade)</t>
-  </si>
-  <si>
-    <t>Modelagem lógica do projeto v1</t>
-  </si>
-  <si>
-    <t>Script de criação do banco/Tabelas criadas em BD local</t>
-  </si>
-  <si>
-    <t>Simular a integração do sistema (utilização do sensor + gráfico)</t>
-  </si>
-  <si>
-    <t>Usar API local/sensor</t>
-  </si>
-  <si>
     <t>Arquitetura Computacional</t>
   </si>
   <si>
     <t>SP2</t>
   </si>
   <si>
-    <t>Protótipo do site institucional</t>
-  </si>
-  <si>
-    <t>Diagrama de visão de negócio</t>
-  </si>
-  <si>
-    <t>Justificativa do projeto</t>
-  </si>
-  <si>
-    <t>Contexto de negócio</t>
-  </si>
-  <si>
-    <t>Ferramenta de gestão de projeto funcionando</t>
-  </si>
-  <si>
-    <t>Documentação inicial do projeto</t>
-  </si>
-  <si>
-    <t>Execução de script de inserção de registros</t>
-  </si>
-  <si>
-    <t>Execução de script de consulta de dados</t>
-  </si>
-  <si>
-    <t>Rodar código Arduino</t>
-  </si>
-  <si>
-    <t>Setup de client de virtualização</t>
-  </si>
-  <si>
-    <t>Planilha de riscos do projeto</t>
-  </si>
-  <si>
-    <t>Especificação da dashboard</t>
-  </si>
-  <si>
-    <t>Site estático institucional - Local em HTML/CSS/JavaScript</t>
-  </si>
-  <si>
-    <t>Site estático dashboard (Gráfico com ChartJS) - Local</t>
-  </si>
-  <si>
-    <t>Site estático cadastro e login - Local (com conceito de repetições)</t>
-  </si>
-  <si>
-    <t>Diagrama de solução (Arquitetura técnica do projeto)</t>
-  </si>
-  <si>
-    <t>Projeto atualizado no GitHub/Documentação do projeto atualizada</t>
-  </si>
-  <si>
-    <t>Product backlog*</t>
-  </si>
-  <si>
     <t>*Está nos slides de TI, mas não nos de PI</t>
   </si>
   <si>
@@ -207,9 +117,6 @@
     <t>Essencial</t>
   </si>
   <si>
-    <t>Simulador financeiro do grupo</t>
-  </si>
-  <si>
     <t>Tam (#)</t>
   </si>
   <si>
@@ -273,30 +180,6 @@
     <t>Pendente</t>
   </si>
   <si>
-    <t>Site - Sobre nós</t>
-  </si>
-  <si>
-    <t>Site - Calculadora</t>
-  </si>
-  <si>
-    <t>Recuperação de senha</t>
-  </si>
-  <si>
-    <t>Filtro de Categorias</t>
-  </si>
-  <si>
-    <t>Barra de Pesquisa</t>
-  </si>
-  <si>
-    <t>Mapa de Recintos/Sensor</t>
-  </si>
-  <si>
-    <t>Alerta e Notificações</t>
-  </si>
-  <si>
-    <t>Gerar Relatórios</t>
-  </si>
-  <si>
     <t>Opção logo abaixo do formulário de login para recuperar a senha. Ao acessar, solicitar o e-mail registrado. Caso seja encontrado nos registros, um e-mail será enviado ao e-mail cadastrado com instruções para recuperação.</t>
   </si>
   <si>
@@ -318,69 +201,39 @@
     <t>Desejável</t>
   </si>
   <si>
-    <t>Apresentação de slides do projeto, ajustes e preparação</t>
-  </si>
-  <si>
     <t>Definição dos slides, conteúdo, textos, formato e distribuição da apresentação</t>
   </si>
   <si>
-    <t>Criptografia das senhas</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mantendo a segurança dos usuários, criptografando a senha antes do armazenamento no banco de dados </t>
   </si>
   <si>
     <t>Filtro com categorias de seleção por animal, tipo de dado (temperatura ou umidade), recintos e datas.</t>
   </si>
   <si>
-    <t>Botões interativos para locomoção do usuário no site</t>
-  </si>
-  <si>
     <t xml:space="preserve">Botões de navegação intuitivo para facilitar o acesso as funcionalidades e as páginas do site. </t>
   </si>
   <si>
-    <t>Ferramenta de Help Desk</t>
-  </si>
-  <si>
     <t>Sistema de suporte ao cliente para contato com a empresa.</t>
   </si>
   <si>
-    <t>IA para Consultas</t>
-  </si>
-  <si>
     <t>Assistente virtual para consultas rápidas exclusivamente para desenvolvedores para os desenvolvedores.</t>
   </si>
   <si>
-    <t>Fale conosco</t>
-  </si>
-  <si>
     <t>A tela “contato” deve conter meios de contato pelos quais o usuário poderá se comunicar com o suporte.</t>
   </si>
   <si>
     <t>Não funcional</t>
   </si>
   <si>
-    <t>Desempenho</t>
-  </si>
-  <si>
     <t>Atualização rápida e eficiente no site para melhor experiência do usuário.</t>
   </si>
   <si>
-    <t>Responsividade</t>
-  </si>
-  <si>
     <t>Interface intuitiva e visualmente agradável compatível com diferentes dispositivos</t>
   </si>
   <si>
-    <t>Segurança</t>
-  </si>
-  <si>
     <t>Proteção contra acessos não autorizados e perda de dados ou possíveis vulnerabilidades.</t>
   </si>
   <si>
-    <t>Alertas</t>
-  </si>
-  <si>
     <t>Alertas para alterações acima ou abaixo dos limites estabelecidos</t>
   </si>
   <si>
@@ -412,9 +265,6 @@
   </si>
   <si>
     <t>Backlog da sprint com pontuação baseada em Fibonacci.</t>
-  </si>
-  <si>
-    <t>Backlog do sprint com pontuação baseada em Fibonacci.</t>
   </si>
   <si>
     <t>Modelagem das tabelas de banco de dados, com relacionamentos estabelecidos.</t>
@@ -518,21 +368,12 @@
     <t>SP2.4</t>
   </si>
   <si>
-    <t>Validação com a Vivian</t>
-  </si>
-  <si>
-    <t>Site institucional revamp</t>
-  </si>
-  <si>
     <t>Alterar o site com base nas alterações no protótipo</t>
   </si>
   <si>
     <t>Checar detalhes referentes a modelagem do banco de dados</t>
   </si>
   <si>
-    <t>Validar Diagrama da solução técnica</t>
-  </si>
-  <si>
     <t>Checar se diagrama da solução técnica está de acordo com o modelo de ISO</t>
   </si>
   <si>
@@ -540,6 +381,177 @@
   </si>
   <si>
     <t>SP3</t>
+  </si>
+  <si>
+    <t>Pesquisa de novos dados para inclusão na documentaçã do projeto</t>
+  </si>
+  <si>
+    <t>Desenvolvimento das regras do grupo para a realização do projeto</t>
+  </si>
+  <si>
+    <t>Backlog do produto com pontuação baseada em Fibonacci.</t>
+  </si>
+  <si>
+    <t>ESP1 - Projeto criado e configrado no GitHub</t>
+  </si>
+  <si>
+    <t>ESP1 - Contexto de negócio</t>
+  </si>
+  <si>
+    <t>ESP1 - Justificativa do projeto</t>
+  </si>
+  <si>
+    <t>ESP1 - Diagrama de visão de negócio</t>
+  </si>
+  <si>
+    <t>ESP1 - Protótipo do site institucional</t>
+  </si>
+  <si>
+    <t>ESP1 - Tela de simulador financeiro (individual)</t>
+  </si>
+  <si>
+    <t>ESP1 - Ferramenta de gestão de projeto funcionando</t>
+  </si>
+  <si>
+    <t>ESP1 - Requisitos populados na ferramenta</t>
+  </si>
+  <si>
+    <t>ESP1 - Documentação inicial do projeto</t>
+  </si>
+  <si>
+    <t>ESP1 - Tabelas criadas no MySQL - Protótipo individual</t>
+  </si>
+  <si>
+    <t>ESP1 - Execução de script de inserção de registros</t>
+  </si>
+  <si>
+    <t>ESP1 - Execução de script de consulta de dados</t>
+  </si>
+  <si>
+    <t>ESP1 - Ligar Arduino</t>
+  </si>
+  <si>
+    <t>ESP1 - Rodar código Arduino</t>
+  </si>
+  <si>
+    <t>ESP1 - Setup de client de virtualização</t>
+  </si>
+  <si>
+    <t>ESP1 - Linux instalado em VM local</t>
+  </si>
+  <si>
+    <t>ESP2.1 - Projeto atualizado no GitHub/Documentação do projeto atualizada</t>
+  </si>
+  <si>
+    <t>ESP2.1 - Script de criação do banco/Tabelas criadas em BD local</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Planilha de riscos do projeto</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Atividades organizadas na ferramenta de gestão (Sprints/Atividades)</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Simular a integração do sistema (utilização do sensor + gráfico)</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Usar API local/sensor</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Site estático institucional - Local em HTML/CSS/JavaScript</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Diagrama de solução (Arquitetura técnica do projeto)</t>
+  </si>
+  <si>
+    <t>ESP2.2 - Modelagem lógica do projeto v1</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Simulador financeiro do grupo</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Especificação da dashboard</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Site estático dashboard (Gráfico com ChartJS) - Local</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Site estático cadastro e login - Local (com conceito de repetições)</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Backlog da sprint (Demanda, pontuação, prioridade)</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Product backlog*</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Site - Sobre nós</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Site - Calculadora</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Site institucional revamp</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Validação da modelagem com a Vivian</t>
+  </si>
+  <si>
+    <t>ESP2.3 - Validar Diagrama da solução técnica</t>
+  </si>
+  <si>
+    <t>ESP2.4 - Apresentação de slides do projeto, ajustes e preparação</t>
+  </si>
+  <si>
+    <t>RSP3 - Recuperação de senha</t>
+  </si>
+  <si>
+    <t>RSP3 - Filtro de Categorias</t>
+  </si>
+  <si>
+    <t>RSP3 - Barra de Pesquisa</t>
+  </si>
+  <si>
+    <t>RSP3 - Mapa de Recintos/Sensor</t>
+  </si>
+  <si>
+    <t>RSP3 - Alerta e Notificações</t>
+  </si>
+  <si>
+    <t>RSP3 - Gerar Relatórios</t>
+  </si>
+  <si>
+    <t>RSP3 - Criptografia das senhas</t>
+  </si>
+  <si>
+    <t>RSP3 - Botões interativos para locomoção do usuário no site</t>
+  </si>
+  <si>
+    <t>RSP3 - Ferramenta de Help Desk</t>
+  </si>
+  <si>
+    <t>RSP3 - IA para Consultas</t>
+  </si>
+  <si>
+    <t>RSP3 - Fale conosco</t>
+  </si>
+  <si>
+    <t>RSP3 - Desempenho</t>
+  </si>
+  <si>
+    <t>RSP3 - Responsividade</t>
+  </si>
+  <si>
+    <t>RSP3 - Segurança</t>
+  </si>
+  <si>
+    <t>RSP3 - Alertas</t>
+  </si>
+  <si>
+    <t>ESP2.1 - Reformulação do contexto do projeto</t>
+  </si>
+  <si>
+    <t>ESP2.1 - Regras do grupo</t>
   </si>
 </sst>
 </file>
@@ -1081,11 +1093,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
-  <dimension ref="B1:L55"/>
+  <dimension ref="B1:L59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.1" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -1107,1920 +1119,1994 @@
   <sheetData>
     <row r="1" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F2" s="4">
         <f>IFERROR(VLOOKUP(E2,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4">
         <f>IFERROR(VLOOKUP(E3,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>25</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4">
         <f>IFERROR(VLOOKUP(E4,Fibonacci!D:E,2,0),"")</f>
         <v>3</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>24</v>
+        <v>114</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4">
         <f>IFERROR(VLOOKUP(E5,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F6" s="4">
         <f>IFERROR(VLOOKUP(E6,Fibonacci!D:E,2,0),"")</f>
         <v>13</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F7" s="4">
         <f>IFERROR(VLOOKUP(E7,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F8" s="4">
         <f>IFERROR(VLOOKUP(E8,Fibonacci!D:E,2,0),"")</f>
         <v>3</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F9" s="4">
         <f>IFERROR(VLOOKUP(E9,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F10" s="4">
         <f>IFERROR(VLOOKUP(E10,Fibonacci!D:E,2,0),"")</f>
         <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F11" s="4">
         <f>IFERROR(VLOOKUP(E11,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4">
         <f>IFERROR(VLOOKUP(E12,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>30</v>
+        <v>122</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F13" s="4">
         <f>IFERROR(VLOOKUP(E13,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F14" s="4">
         <f>IFERROR(VLOOKUP(E14,Fibonacci!D:E,2,0),"")</f>
         <v>3</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F15" s="4">
         <f>IFERROR(VLOOKUP(E15,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F16" s="4">
         <f>IFERROR(VLOOKUP(E16,Fibonacci!D:E,2,0),"")</f>
         <v>3</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F17" s="4">
         <f>IFERROR(VLOOKUP(E17,Fibonacci!D:E,2,0),"")</f>
         <v>3</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F18" s="4">
         <f>IFERROR(VLOOKUP(E18,Fibonacci!D:E,2,0),"")</f>
         <v>3</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F19" s="4">
         <f>IFERROR(VLOOKUP(E19,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="F20" s="4">
         <f>IFERROR(VLOOKUP(E20,Fibonacci!D:E,2,0),"")</f>
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="F21" s="4">
         <f>IFERROR(VLOOKUP(E21,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>126</v>
+        <v>65</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="F22" s="4">
         <f>IFERROR(VLOOKUP(E22,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F23" s="4">
         <f>IFERROR(VLOOKUP(E23,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F24" s="4">
         <f>IFERROR(VLOOKUP(E24,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>38</v>
+        <v>132</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F25" s="4">
         <f>IFERROR(VLOOKUP(E25,Fibonacci!D:E,2,0),"")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>124</v>
+        <v>68</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F26" s="4">
         <f>IFERROR(VLOOKUP(E26,Fibonacci!D:E,2,0),"")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>150</v>
+        <v>98</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>54</v>
+        <v>134</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F27" s="4">
         <f>IFERROR(VLOOKUP(E27,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="F28" s="4">
         <f>IFERROR(VLOOKUP(E28,Fibonacci!D:E,2,0),"")</f>
         <v>5</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>146</v>
+        <v>97</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>118</v>
+        <v>32</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="F29" s="4">
         <f>IFERROR(VLOOKUP(E29,Fibonacci!D:E,2,0),"")</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>37</v>
+        <v>137</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F30" s="4">
         <f>IFERROR(VLOOKUP(E30,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>122</v>
+        <v>69</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F31" s="4">
         <f>IFERROR(VLOOKUP(E31,Fibonacci!D:E,2,0),"")</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>123</v>
+        <v>70</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F32" s="4">
         <f>IFERROR(VLOOKUP(E32,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="8" t="s">
-        <v>76</v>
+        <v>140</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F33" s="4">
         <f>IFERROR(VLOOKUP(E33,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F34" s="4">
         <f>IFERROR(VLOOKUP(E34,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>4</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="8" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>155</v>
+        <v>78</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F35" s="4">
         <f>IFERROR(VLOOKUP(E35,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>156</v>
+        <v>79</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="F36" s="4">
         <f>IFERROR(VLOOKUP(E36,Fibonacci!D:E,2,0),"")</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="8" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>158</v>
+        <v>103</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="F37" s="4">
         <f>IFERROR(VLOOKUP(E37,Fibonacci!D:E,2,0),"")</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="F38" s="4">
         <f>IFERROR(VLOOKUP(E38,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="8" t="s">
-        <v>78</v>
+        <v>146</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="F39" s="4">
         <f>IFERROR(VLOOKUP(E39,Fibonacci!D:E,2,0),"")</f>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>113</v>
+        <v>6</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="K39" s="4" t="s">
-        <v>160</v>
+        <v>96</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="F40" s="4">
         <f>IFERROR(VLOOKUP(E40,Fibonacci!D:E,2,0),"")</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>113</v>
+        <v>2</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>131</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="8" t="s">
-        <v>80</v>
+        <v>148</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="F41" s="4">
         <f>IFERROR(VLOOKUP(E41,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F42" s="4">
         <f>IFERROR(VLOOKUP(E42,Fibonacci!D:E,2,0),"")</f>
         <v>13</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="8" t="s">
-        <v>82</v>
+        <v>150</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F43" s="4">
         <f>IFERROR(VLOOKUP(E43,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="8" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="F44" s="4">
         <f>IFERROR(VLOOKUP(E44,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="8" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="F45" s="4">
         <f>IFERROR(VLOOKUP(E45,Fibonacci!D:E,2,0),"")</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="8" t="s">
-        <v>96</v>
+        <v>153</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="F46" s="4">
         <f>IFERROR(VLOOKUP(E46,Fibonacci!D:E,2,0),"")</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="8" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F47" s="4">
         <f>IFERROR(VLOOKUP(E47,Fibonacci!D:E,2,0),"")</f>
         <v>13</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="8" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F48" s="4">
         <f>IFERROR(VLOOKUP(E48,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="8" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F49" s="4">
         <f>IFERROR(VLOOKUP(E49,Fibonacci!D:E,2,0),"")</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="8" t="s">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F50" s="4">
         <f>IFERROR(VLOOKUP(E50,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="8" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="F51" s="4">
         <f>IFERROR(VLOOKUP(E51,Fibonacci!D:E,2,0),"")</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="8" t="s">
-        <v>109</v>
+        <v>159</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="F52" s="4">
         <f>IFERROR(VLOOKUP(E52,Fibonacci!D:E,2,0),"")</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="8" t="s">
-        <v>111</v>
+        <v>160</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F53" s="4">
         <f>IFERROR(VLOOKUP(E53,Fibonacci!D:E,2,0),"")</f>
         <v>8</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>148</v>
+        <v>99</v>
       </c>
       <c r="H53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="K53" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="L53" s="4" t="s">
-        <v>131</v>
+      <c r="E54" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" s="4">
+        <f>IFERROR(VLOOKUP(E54,Fibonacci!D:E,2,0),"")</f>
+        <v>13</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I54" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L54" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
+      <c r="B55" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="4">
+        <f>IFERROR(VLOOKUP(E55,Fibonacci!D:E,2,0),"")</f>
+        <v>8</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="B1:L53" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L53">
-      <sortCondition ref="K1:K53"/>
+  <autoFilter ref="B1:L55" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:L55">
+      <sortCondition ref="K1:K55"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="L1:L1048576">
@@ -3038,7 +3124,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A5EF24D9-CB2D-4BDC-89A1-7AFACDE7C990}">
           <x14:formula1>
             <xm:f>Fibonacci!$D$7:$D$11</xm:f>
@@ -3056,7 +3142,7 @@
   <dimension ref="F7:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3067,12 +3153,12 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>159</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G9" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F9,'Product Backlog'!F:F)</f>
@@ -3081,16 +3167,16 @@
     </row>
     <row r="10" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F10" s="5" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="G10" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F10,'Product Backlog'!F:F)</f>
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F11" s="5" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="G11" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F11,'Product Backlog'!F:F)</f>
@@ -3099,7 +3185,7 @@
     </row>
     <row r="12" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F12" s="5" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="G12" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F12,'Product Backlog'!F:F)</f>
@@ -3108,7 +3194,7 @@
     </row>
     <row r="13" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F13" s="5" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="G13" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F13,'Product Backlog'!F:F)</f>
@@ -3117,7 +3203,7 @@
     </row>
     <row r="14" spans="6:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F14" s="9" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="G14" s="5">
         <f>SUMIF('Product Backlog'!K:K,'Fibonacci por Sprint'!F14,'Product Backlog'!F:F)</f>
@@ -3146,50 +3232,50 @@
     <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3197,15 +3283,15 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3213,15 +3299,15 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3267,60 +3353,60 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -3345,7 +3431,7 @@
   <dimension ref="D5:E12"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E11"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3357,15 +3443,15 @@
     <row r="5" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="4:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="4:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5">
         <v>3</v>
@@ -3373,7 +3459,7 @@
     </row>
     <row r="8" spans="4:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="5" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5">
         <v>5</v>
@@ -3381,7 +3467,7 @@
     </row>
     <row r="9" spans="4:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="5" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5">
         <v>8</v>
@@ -3389,7 +3475,7 @@
     </row>
     <row r="10" spans="4:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="5" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E10" s="5">
         <v>13</v>
@@ -3397,7 +3483,7 @@
     </row>
     <row r="11" spans="4:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="5" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="E11" s="5">
         <v>21</v>

</xml_diff>

<commit_message>
docs: adição do project patterns
</commit_message>
<xml_diff>
--- a/Backlog HerpSafe/Produck backlog.xlsx
+++ b/Backlog HerpSafe/Produck backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - SPTech School\202501\Pesquisa e Inovação\Sprint 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezequiel\Downloads\HerpSafe-Sprint-2\Backlog HerpSafe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08E89BF6-0D29-46CE-9988-B0863E024C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813BBE0B-4DB8-4001-A0C0-6ADCAB413461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10440" windowHeight="10905" xr2:uid="{AB679324-3DC8-4F8A-B107-B10CD92536BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="3" r:id="rId1"/>
@@ -665,7 +665,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1095,9 +1095,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{831A3FE2-A405-481B-8C5B-5096A2CC35E1}">
   <dimension ref="B1:L59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.1" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -3142,7 +3142,7 @@
   <dimension ref="F7:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3221,7 +3221,7 @@
   <dimension ref="B3:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>